<commit_message>
Added tests for mailmerge_factory in utility.py
</commit_message>
<xml_diff>
--- a/data/tests/test_data_source.xlsx
+++ b/data/tests/test_data_source.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC62AAB-4C12-7F4F-AAC5-857DCB749C37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31EC618-6D8A-F748-8D9A-72FF3014061F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="5020" windowWidth="26180" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4820" yWindow="5020" windowWidth="26180" windowHeight="16460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_data" sheetId="1" r:id="rId1"/>
     <sheet name="project_data_single_1" sheetId="2" r:id="rId2"/>
     <sheet name="project_data_single_2" sheetId="4" r:id="rId3"/>
     <sheet name="project_data_multiple" sheetId="3" r:id="rId4"/>
+    <sheet name="empty" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -625,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="167" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1198,4 +1199,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1F1F30-03F9-694D-AFB7-16BF524B6F3B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>